<commit_message>
Update a_psat views, models, templates, study_data
</commit_message>
<xml_diff>
--- a/a_psat/data/study_data.xlsx
+++ b/a_psat/data/study_data.xlsx
@@ -8,25 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\paedison3\a_psat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6B190F-2F7D-451B-BF18-362E89A42F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA7D926-4C27-4B61-AA7E-3D728979AAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-54720" yWindow="2220" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="problem" sheetId="2" r:id="rId1"/>
     <sheet name="student" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2159" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="102">
   <si>
     <t>year</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -310,6 +321,43 @@
   <si>
     <t>심화</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>우은주</t>
+  </si>
+  <si>
+    <t>이윤서</t>
+  </si>
+  <si>
+    <t>장아연</t>
+  </si>
+  <si>
+    <t>천의성</t>
+  </si>
+  <si>
+    <t>문소원</t>
+  </si>
+  <si>
+    <t>박초이</t>
+  </si>
+  <si>
+    <t>이현주</t>
+  </si>
+  <si>
+    <t>정승호</t>
+  </si>
+  <si>
+    <t>최수연</t>
+  </si>
+  <si>
+    <t>김윤진</t>
+  </si>
+  <si>
+    <t>박형진</t>
+  </si>
+  <si>
+    <t>프라임</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -669,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DAF1E21-CF0C-421D-9ED1-AC0472BE1C95}">
   <dimension ref="A1:H671"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A552" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A516" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -18133,10 +18181,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -19314,6 +19362,193 @@
         <v>72</v>
       </c>
     </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>2021</v>
+      </c>
+      <c r="B70" t="s">
+        <v>101</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>2021</v>
+      </c>
+      <c r="B71" t="s">
+        <v>101</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>2021</v>
+      </c>
+      <c r="B72" t="s">
+        <v>101</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>2021</v>
+      </c>
+      <c r="B73" t="s">
+        <v>101</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>4</v>
+      </c>
+      <c r="E73" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>2021</v>
+      </c>
+      <c r="B74" t="s">
+        <v>101</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>5</v>
+      </c>
+      <c r="E74" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>2021</v>
+      </c>
+      <c r="B75" t="s">
+        <v>101</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>6</v>
+      </c>
+      <c r="E75" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>2021</v>
+      </c>
+      <c r="B76" t="s">
+        <v>101</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>7</v>
+      </c>
+      <c r="E76" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>2021</v>
+      </c>
+      <c r="B77" t="s">
+        <v>101</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>8</v>
+      </c>
+      <c r="E77" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>2021</v>
+      </c>
+      <c r="B78" t="s">
+        <v>101</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>9</v>
+      </c>
+      <c r="E78" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>2021</v>
+      </c>
+      <c r="B79" t="s">
+        <v>101</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>10</v>
+      </c>
+      <c r="E79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>2021</v>
+      </c>
+      <c r="B80" t="s">
+        <v>101</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>11</v>
+      </c>
+      <c r="E80" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>